<commit_message>
updated to latest config
</commit_message>
<xml_diff>
--- a/Assets/counter-3.xlsx
+++ b/Assets/counter-3.xlsx
@@ -7,17 +7,18 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-10" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-09" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-08" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-07" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-06" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-05" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-04" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-03" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-02" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="28 Feb 20 -- 05 Mar 20" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="24 Feb 20 -- 01 Mar 20" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="28 Mar 20 -- 03 Apr 20" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-10" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-09" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-08" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-07" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-06" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-05" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-04" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-03" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-03-02" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="28 Feb 20 -- 05 Mar 20" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="24 Feb 20 -- 01 Mar 20" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
@@ -398,45 +399,30 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Total Count</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>AD/RES</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>473</t>
-        </is>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Civ</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>159</t>
-        </is>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Ret</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>168</t>
         </is>
       </c>
     </row>
@@ -457,7 +443,7 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="2" width="8.67"/>
   </cols>
@@ -477,7 +463,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>337</t>
         </is>
       </c>
     </row>
@@ -489,7 +475,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>130</t>
         </is>
       </c>
     </row>
@@ -501,7 +487,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>154</t>
         </is>
       </c>
     </row>
@@ -513,6 +499,73 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="2" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="3">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Total Count</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="2" s="3">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AD/RES</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="3" s="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Civ</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="4" s="3">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Ret</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -524,7 +577,7 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="2" width="8.67"/>
   </cols>
@@ -593,7 +646,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>474</t>
+          <t>473</t>
         </is>
       </c>
     </row>
@@ -605,7 +658,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -617,7 +670,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>159</t>
+          <t>168</t>
         </is>
       </c>
     </row>
@@ -655,7 +708,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>235</t>
+          <t>474</t>
         </is>
       </c>
     </row>
@@ -667,7 +720,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>169</t>
         </is>
       </c>
     </row>
@@ -679,7 +732,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>159</t>
         </is>
       </c>
     </row>
@@ -717,7 +770,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>235</t>
         </is>
       </c>
     </row>
@@ -729,7 +782,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>64</t>
         </is>
       </c>
     </row>
@@ -741,7 +794,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>56</t>
         </is>
       </c>
     </row>
@@ -779,7 +832,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>393</t>
+          <t>207</t>
         </is>
       </c>
     </row>
@@ -791,7 +844,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>113</t>
         </is>
       </c>
     </row>
@@ -803,7 +856,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>101</t>
         </is>
       </c>
     </row>
@@ -841,7 +894,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>452</t>
+          <t>393</t>
         </is>
       </c>
     </row>
@@ -853,7 +906,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>129</t>
         </is>
       </c>
     </row>
@@ -865,7 +918,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>121</t>
         </is>
       </c>
     </row>
@@ -903,7 +956,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>452</t>
         </is>
       </c>
     </row>
@@ -915,7 +968,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>121</t>
         </is>
       </c>
     </row>
@@ -927,7 +980,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>145</t>
         </is>
       </c>
     </row>
@@ -937,6 +990,68 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Total Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AD/RES</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>403</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Civ</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>146</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Ret</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -948,7 +1063,7 @@
       <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="2" width="8.67"/>
   </cols>
@@ -1001,71 +1116,4 @@
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
   <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
-  <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row customHeight="1" ht="15" r="1" s="3">
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Total Count</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2" s="3">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>AD/RES</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>337</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="3" s="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Civ</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="4" s="3">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Ret</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>154</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>